<commit_message>
Generate boiler lookup from excel.
</commit_message>
<xml_diff>
--- a/conf/steamworks_boiler_data.xlsx
+++ b/conf/steamworks_boiler_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27860" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27840" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -402,650 +402,1820 @@
       <c r="A3">
         <v>71</v>
       </c>
+      <c r="B3">
+        <v>199</v>
+      </c>
+      <c r="C3">
+        <v>85</v>
+      </c>
+      <c r="D3">
+        <v>100</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>72</v>
       </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>73</v>
       </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>74</v>
       </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>75</v>
       </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>76</v>
       </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>77</v>
       </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>78</v>
       </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>79</v>
       </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>80</v>
       </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>81</v>
       </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>82</v>
       </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>83</v>
       </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>84</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>85</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>86</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>87</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>88</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>89</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>90</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>91</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>92</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>93</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>94</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>95</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>96</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>97</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>98</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>99</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>100</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>101</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>102</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>103</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B35">
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>104</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B36">
+        <v>0</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>105</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B37">
+        <v>0</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>106</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B38">
+        <v>0</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>107</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B39">
+        <v>0</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>108</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B40">
+        <v>0</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>109</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B41">
+        <v>0</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>110</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B42">
+        <v>0</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>111</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B43">
+        <v>0</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>112</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B44">
+        <v>0</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>113</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B45">
+        <v>0</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>114</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B46">
+        <v>0</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>115</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B47">
+        <v>0</v>
+      </c>
+      <c r="C47">
+        <v>0</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>116</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B48">
+        <v>0</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>117</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B49">
+        <v>0</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>118</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B50">
+        <v>0</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>119</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B51">
+        <v>0</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>120</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B52">
+        <v>0</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>121</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B53">
+        <v>0</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>122</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B54">
+        <v>0</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>123</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B55">
+        <v>0</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>124</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B56">
+        <v>0</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>125</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B57">
+        <v>0</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>126</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B58">
+        <v>0</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>127</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B59">
+        <v>0</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>128</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B60">
+        <v>0</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>129</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B61">
+        <v>0</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>130</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B62">
+        <v>0</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>131</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B63">
+        <v>0</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>132</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B64">
+        <v>0</v>
+      </c>
+      <c r="C64">
+        <v>0</v>
+      </c>
+      <c r="D64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>133</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B65">
+        <v>0</v>
+      </c>
+      <c r="C65">
+        <v>0</v>
+      </c>
+      <c r="D65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>134</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B66">
+        <v>0</v>
+      </c>
+      <c r="C66">
+        <v>0</v>
+      </c>
+      <c r="D66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>135</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B67">
+        <v>0</v>
+      </c>
+      <c r="C67">
+        <v>0</v>
+      </c>
+      <c r="D67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>136</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B68">
+        <v>0</v>
+      </c>
+      <c r="C68">
+        <v>0</v>
+      </c>
+      <c r="D68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>137</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B69">
+        <v>0</v>
+      </c>
+      <c r="C69">
+        <v>0</v>
+      </c>
+      <c r="D69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>138</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B70">
+        <v>0</v>
+      </c>
+      <c r="C70">
+        <v>0</v>
+      </c>
+      <c r="D70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>139</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B71">
+        <v>0</v>
+      </c>
+      <c r="C71">
+        <v>0</v>
+      </c>
+      <c r="D71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>140</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B72">
+        <v>0</v>
+      </c>
+      <c r="C72">
+        <v>0</v>
+      </c>
+      <c r="D72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>141</v>
       </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B73">
+        <v>0</v>
+      </c>
+      <c r="C73">
+        <v>0</v>
+      </c>
+      <c r="D73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>142</v>
       </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B74">
+        <v>0</v>
+      </c>
+      <c r="C74">
+        <v>0</v>
+      </c>
+      <c r="D74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>143</v>
       </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B75">
+        <v>0</v>
+      </c>
+      <c r="C75">
+        <v>0</v>
+      </c>
+      <c r="D75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>144</v>
       </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B76">
+        <v>0</v>
+      </c>
+      <c r="C76">
+        <v>0</v>
+      </c>
+      <c r="D76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>145</v>
       </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B77">
+        <v>0</v>
+      </c>
+      <c r="C77">
+        <v>0</v>
+      </c>
+      <c r="D77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>146</v>
       </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B78">
+        <v>0</v>
+      </c>
+      <c r="C78">
+        <v>0</v>
+      </c>
+      <c r="D78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>147</v>
       </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B79">
+        <v>0</v>
+      </c>
+      <c r="C79">
+        <v>0</v>
+      </c>
+      <c r="D79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>148</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B80">
+        <v>0</v>
+      </c>
+      <c r="C80">
+        <v>0</v>
+      </c>
+      <c r="D80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>149</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B81">
+        <v>0</v>
+      </c>
+      <c r="C81">
+        <v>0</v>
+      </c>
+      <c r="D81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>150</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B82">
+        <v>0</v>
+      </c>
+      <c r="C82">
+        <v>0</v>
+      </c>
+      <c r="D82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>151</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B83">
+        <v>0</v>
+      </c>
+      <c r="C83">
+        <v>0</v>
+      </c>
+      <c r="D83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>152</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B84">
+        <v>0</v>
+      </c>
+      <c r="C84">
+        <v>0</v>
+      </c>
+      <c r="D84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>153</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B85">
+        <v>0</v>
+      </c>
+      <c r="C85">
+        <v>0</v>
+      </c>
+      <c r="D85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>154</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B86">
+        <v>0</v>
+      </c>
+      <c r="C86">
+        <v>0</v>
+      </c>
+      <c r="D86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>155</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B87">
+        <v>0</v>
+      </c>
+      <c r="C87">
+        <v>0</v>
+      </c>
+      <c r="D87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>156</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B88">
+        <v>0</v>
+      </c>
+      <c r="C88">
+        <v>0</v>
+      </c>
+      <c r="D88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>157</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B89">
+        <v>0</v>
+      </c>
+      <c r="C89">
+        <v>0</v>
+      </c>
+      <c r="D89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>158</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B90">
+        <v>0</v>
+      </c>
+      <c r="C90">
+        <v>0</v>
+      </c>
+      <c r="D90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>159</v>
       </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B91">
+        <v>0</v>
+      </c>
+      <c r="C91">
+        <v>0</v>
+      </c>
+      <c r="D91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>160</v>
       </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B92">
+        <v>0</v>
+      </c>
+      <c r="C92">
+        <v>0</v>
+      </c>
+      <c r="D92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>161</v>
       </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B93">
+        <v>0</v>
+      </c>
+      <c r="C93">
+        <v>0</v>
+      </c>
+      <c r="D93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>162</v>
       </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B94">
+        <v>0</v>
+      </c>
+      <c r="C94">
+        <v>0</v>
+      </c>
+      <c r="D94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>163</v>
       </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B95">
+        <v>0</v>
+      </c>
+      <c r="C95">
+        <v>0</v>
+      </c>
+      <c r="D95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>164</v>
       </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B96">
+        <v>0</v>
+      </c>
+      <c r="C96">
+        <v>0</v>
+      </c>
+      <c r="D96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>165</v>
       </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B97">
+        <v>0</v>
+      </c>
+      <c r="C97">
+        <v>0</v>
+      </c>
+      <c r="D97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>166</v>
       </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B98">
+        <v>0</v>
+      </c>
+      <c r="C98">
+        <v>0</v>
+      </c>
+      <c r="D98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>167</v>
       </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B99">
+        <v>0</v>
+      </c>
+      <c r="C99">
+        <v>0</v>
+      </c>
+      <c r="D99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>168</v>
       </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B100">
+        <v>0</v>
+      </c>
+      <c r="C100">
+        <v>0</v>
+      </c>
+      <c r="D100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>169</v>
       </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B101">
+        <v>0</v>
+      </c>
+      <c r="C101">
+        <v>0</v>
+      </c>
+      <c r="D101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>170</v>
       </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B102">
+        <v>0</v>
+      </c>
+      <c r="C102">
+        <v>0</v>
+      </c>
+      <c r="D102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>171</v>
       </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B103">
+        <v>0</v>
+      </c>
+      <c r="C103">
+        <v>0</v>
+      </c>
+      <c r="D103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>172</v>
       </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B104">
+        <v>0</v>
+      </c>
+      <c r="C104">
+        <v>0</v>
+      </c>
+      <c r="D104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>173</v>
       </c>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B105">
+        <v>0</v>
+      </c>
+      <c r="C105">
+        <v>0</v>
+      </c>
+      <c r="D105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>174</v>
       </c>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B106">
+        <v>0</v>
+      </c>
+      <c r="C106">
+        <v>0</v>
+      </c>
+      <c r="D106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>175</v>
       </c>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B107">
+        <v>0</v>
+      </c>
+      <c r="C107">
+        <v>0</v>
+      </c>
+      <c r="D107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>176</v>
       </c>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B108">
+        <v>0</v>
+      </c>
+      <c r="C108">
+        <v>0</v>
+      </c>
+      <c r="D108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>177</v>
       </c>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B109">
+        <v>0</v>
+      </c>
+      <c r="C109">
+        <v>0</v>
+      </c>
+      <c r="D109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>178</v>
       </c>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B110">
+        <v>0</v>
+      </c>
+      <c r="C110">
+        <v>0</v>
+      </c>
+      <c r="D110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>179</v>
       </c>
-    </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B111">
+        <v>0</v>
+      </c>
+      <c r="C111">
+        <v>0</v>
+      </c>
+      <c r="D111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>180</v>
       </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B112">
+        <v>0</v>
+      </c>
+      <c r="C112">
+        <v>0</v>
+      </c>
+      <c r="D112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>181</v>
       </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B113">
+        <v>0</v>
+      </c>
+      <c r="C113">
+        <v>0</v>
+      </c>
+      <c r="D113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>182</v>
       </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B114">
+        <v>0</v>
+      </c>
+      <c r="C114">
+        <v>0</v>
+      </c>
+      <c r="D114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>183</v>
       </c>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B115">
+        <v>0</v>
+      </c>
+      <c r="C115">
+        <v>0</v>
+      </c>
+      <c r="D115">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>184</v>
       </c>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B116">
+        <v>0</v>
+      </c>
+      <c r="C116">
+        <v>0</v>
+      </c>
+      <c r="D116">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>185</v>
       </c>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B117">
+        <v>0</v>
+      </c>
+      <c r="C117">
+        <v>0</v>
+      </c>
+      <c r="D117">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>186</v>
       </c>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B118">
+        <v>0</v>
+      </c>
+      <c r="C118">
+        <v>0</v>
+      </c>
+      <c r="D118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>187</v>
       </c>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B119">
+        <v>0</v>
+      </c>
+      <c r="C119">
+        <v>0</v>
+      </c>
+      <c r="D119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>188</v>
       </c>
-    </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B120">
+        <v>0</v>
+      </c>
+      <c r="C120">
+        <v>0</v>
+      </c>
+      <c r="D120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>189</v>
       </c>
-    </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B121">
+        <v>0</v>
+      </c>
+      <c r="C121">
+        <v>0</v>
+      </c>
+      <c r="D121">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>190</v>
       </c>
-    </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B122">
+        <v>0</v>
+      </c>
+      <c r="C122">
+        <v>0</v>
+      </c>
+      <c r="D122">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>191</v>
       </c>
-    </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B123">
+        <v>0</v>
+      </c>
+      <c r="C123">
+        <v>0</v>
+      </c>
+      <c r="D123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>192</v>
       </c>
-    </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B124">
+        <v>0</v>
+      </c>
+      <c r="C124">
+        <v>0</v>
+      </c>
+      <c r="D124">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>193</v>
       </c>
-    </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B125">
+        <v>0</v>
+      </c>
+      <c r="C125">
+        <v>0</v>
+      </c>
+      <c r="D125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>194</v>
       </c>
-    </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B126">
+        <v>0</v>
+      </c>
+      <c r="C126">
+        <v>0</v>
+      </c>
+      <c r="D126">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>195</v>
       </c>
-    </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B127">
+        <v>0</v>
+      </c>
+      <c r="C127">
+        <v>0</v>
+      </c>
+      <c r="D127">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>196</v>
       </c>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B128">
+        <v>0</v>
+      </c>
+      <c r="C128">
+        <v>0</v>
+      </c>
+      <c r="D128">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>197</v>
       </c>
-    </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B129">
+        <v>0</v>
+      </c>
+      <c r="C129">
+        <v>0</v>
+      </c>
+      <c r="D129">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>198</v>
       </c>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B130">
+        <v>0</v>
+      </c>
+      <c r="C130">
+        <v>0</v>
+      </c>
+      <c r="D130">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>199</v>
       </c>
-    </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B131">
+        <v>0</v>
+      </c>
+      <c r="C131">
+        <v>0</v>
+      </c>
+      <c r="D131">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>200</v>
+      </c>
+      <c r="B132">
+        <v>99</v>
+      </c>
+      <c r="C132">
+        <v>199</v>
+      </c>
+      <c r="D132">
+        <v>299</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reimplement ranging method to angle measurement.
</commit_message>
<xml_diff>
--- a/conf/steamworks_boiler_data.xlsx
+++ b/conf/steamworks_boiler_data.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28016"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27840" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28720" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -365,7 +365,10 @@
   <dimension ref="A1:D132"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -599,7 +602,7 @@
         <v>85</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>144</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -655,7 +658,7 @@
         <v>89</v>
       </c>
       <c r="B21">
-        <v>0</v>
+        <v>132</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -711,7 +714,7 @@
         <v>93</v>
       </c>
       <c r="B25">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -753,7 +756,7 @@
         <v>96</v>
       </c>
       <c r="B28">
-        <v>0</v>
+        <v>108</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -809,7 +812,7 @@
         <v>100</v>
       </c>
       <c r="B32">
-        <v>0</v>
+        <v>96</v>
       </c>
       <c r="C32">
         <v>0</v>
@@ -837,7 +840,7 @@
         <v>102</v>
       </c>
       <c r="B34">
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="C34">
         <v>0</v>
@@ -2220,5 +2223,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>